<commit_message>
update of SNOW sclasses
in addition: table in pprovider set from uint 8 to unit32, solves problem that classs in the bottom part of large Excel files don't get read
</commit_message>
<xml_diff>
--- a/results/example1/example1.xlsx
+++ b/results/example1/example1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="185">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -552,6 +552,33 @@
   </si>
   <si>
     <t>deltaT</t>
+  </si>
+  <si>
+    <t>SNOW_simple_bucketW_seb</t>
+  </si>
+  <si>
+    <t>max_albedo</t>
+  </si>
+  <si>
+    <t>min_albedo</t>
+  </si>
+  <si>
+    <t>tau_1</t>
+  </si>
+  <si>
+    <t>tau_a</t>
+  </si>
+  <si>
+    <t>tau_f</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>SNOW_simple_seb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">area of the </t>
   </si>
 </sst>
 </file>
@@ -894,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H314"/>
+  <dimension ref="A1:H353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,257 +1305,245 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B40">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>0</v>
-      </c>
-      <c r="B51">
-        <v>0.05</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>0.1</v>
+      </c>
+      <c r="C53">
         <v>2</v>
-      </c>
-      <c r="B53">
-        <v>0.2</v>
-      </c>
-      <c r="C53">
-        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>0.2</v>
+      </c>
+      <c r="C54">
         <v>10</v>
-      </c>
-      <c r="B54">
-        <v>0.5</v>
-      </c>
-      <c r="C54">
-        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>0.5</v>
+      </c>
+      <c r="C55">
         <v>20</v>
       </c>
-      <c r="B55">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56">
         <v>5</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="B62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H64" s="3" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>0</v>
-      </c>
-      <c r="B66">
-        <v>0.3</v>
-      </c>
-      <c r="C66">
-        <v>0.5</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0.3</v>
-      </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66">
-        <v>500</v>
-      </c>
-      <c r="H66">
-        <v>-0.5</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B67">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C67">
         <v>0.5</v>
@@ -1540,18 +1555,18 @@
         <v>0.3</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="B68">
         <v>0.5</v>
@@ -1566,7 +1581,7 @@
         <v>0.3</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -1576,165 +1591,183 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>34</v>
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>0.5</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0.3</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="B75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>88</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>0</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>10</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>34</v>
       </c>
-      <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>107</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C83" s="8"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
-      </c>
-      <c r="B84" s="4">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" s="4">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B89" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="B90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>0</v>
-      </c>
-      <c r="B94">
-        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B95">
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B96">
         <v>-1</v>
@@ -1742,106 +1775,106 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
+        <v>100</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>5000</v>
       </c>
-      <c r="B98">
+      <c r="B99">
         <v>20</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="6"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B106" s="7">
-        <v>1</v>
-      </c>
-      <c r="C106" s="6"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="6"/>
+      <c r="B107" s="7">
+        <v>1</v>
+      </c>
       <c r="C107" s="6"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C109" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>1</v>
-      </c>
-      <c r="B109">
-        <v>0.15</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B110">
-        <v>0.9</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B111">
-        <v>0.01</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="B112">
-        <v>100</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2461,821 +2494,1205 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>84</v>
-      </c>
-      <c r="B181" s="6">
-        <v>1</v>
-      </c>
-      <c r="C181" s="6">
-        <v>1</v>
-      </c>
-      <c r="D181" t="s">
-        <v>85</v>
+        <v>0</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E181" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B182" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C182" s="6" t="s">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="B182" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C182" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D182" t="s">
+        <v>7</v>
       </c>
       <c r="E182" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B183" s="6">
-        <v>3600</v>
+        <v>50000</v>
       </c>
       <c r="C183" s="6">
-        <v>3600</v>
+        <v>50000</v>
       </c>
       <c r="D183" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>64</v>
-      </c>
-      <c r="B184" s="6">
-        <v>50000</v>
-      </c>
-      <c r="C184" s="6">
-        <v>50000</v>
-      </c>
-      <c r="D184" t="s">
-        <v>8</v>
-      </c>
-      <c r="E184" t="s">
-        <v>14</v>
-      </c>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B185" s="6"/>
+      <c r="A185" t="s">
+        <v>82</v>
+      </c>
+      <c r="B185" s="6">
+        <v>3</v>
+      </c>
       <c r="C185" s="6"/>
+      <c r="E185" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>82</v>
-      </c>
-      <c r="B186" s="6">
-        <v>3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B186" s="6"/>
       <c r="C186" s="6"/>
-      <c r="E186" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>42</v>
-      </c>
       <c r="B187" s="6"/>
-      <c r="C187" s="6"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B189" s="6"/>
+      <c r="A189" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>23</v>
+      <c r="A190" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B191" s="7" t="s">
-        <v>15</v>
+        <v>110</v>
+      </c>
+      <c r="B191" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B192" s="7">
-        <v>1</v>
-      </c>
+      <c r="B192" s="6"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B193" s="6"/>
+      <c r="B193" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D193" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B194" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C194" s="6" t="s">
-        <v>17</v>
+      <c r="A194" t="s">
+        <v>1</v>
+      </c>
+      <c r="B194" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="C194" s="6">
+        <v>0.08</v>
       </c>
       <c r="D194" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="E194" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="B195" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="C195" s="6">
-        <v>0.08</v>
+        <v>2</v>
+      </c>
+      <c r="C195" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D195" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="E195" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="B196" s="6">
-        <v>2</v>
-      </c>
-      <c r="C196" s="6" t="s">
-        <v>112</v>
+        <v>0.99</v>
+      </c>
+      <c r="C196" s="6">
+        <v>0.99</v>
       </c>
       <c r="D196" t="s">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="E196" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B197" s="6">
-        <v>0.99</v>
+        <v>1E-3</v>
       </c>
       <c r="C197" s="6">
-        <v>0.99</v>
+        <v>1E-3</v>
       </c>
       <c r="D197" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E197" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B198" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="C198" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="D198" t="s">
-        <v>6</v>
-      </c>
-      <c r="E198" t="s">
-        <v>12</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C198" s="6"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B199" s="6">
-        <v>0</v>
-      </c>
-      <c r="C199" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="C199" s="6">
+        <v>1</v>
+      </c>
+      <c r="D199" t="s">
+        <v>85</v>
+      </c>
+      <c r="E199" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>84</v>
-      </c>
-      <c r="B200" s="6">
-        <v>10</v>
-      </c>
-      <c r="C200" s="6">
-        <v>1</v>
-      </c>
-      <c r="D200" t="s">
-        <v>85</v>
+        <v>0</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E200" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C201" s="6" t="s">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="B201" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C201" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D201" t="s">
+        <v>7</v>
       </c>
       <c r="E201" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B202" s="6">
-        <v>3600</v>
+        <v>50000</v>
       </c>
       <c r="C202" s="6">
-        <v>3600</v>
+        <v>50000</v>
       </c>
       <c r="D202" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>64</v>
-      </c>
-      <c r="B203" s="6">
-        <v>50000</v>
-      </c>
-      <c r="C203" s="6">
-        <v>50000</v>
-      </c>
-      <c r="D203" t="s">
-        <v>8</v>
-      </c>
-      <c r="E203" t="s">
-        <v>14</v>
-      </c>
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B204" s="6"/>
+      <c r="A204" t="s">
+        <v>115</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="C204" s="6"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>115</v>
-      </c>
-      <c r="B205" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C205" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="B205" s="6"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>42</v>
-      </c>
       <c r="B206" s="6"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
-      <c r="C207" s="6"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B208" s="9"/>
+      <c r="A208" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C208" s="6"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A209" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" s="6"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B210" t="s">
-        <v>15</v>
+        <v>176</v>
+      </c>
+      <c r="B210" s="7">
+        <v>1</v>
       </c>
       <c r="C210" s="6"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B211" s="6">
-        <v>1</v>
-      </c>
+      <c r="B211" s="6"/>
       <c r="C211" s="6"/>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B212" s="6"/>
-      <c r="C212" s="6"/>
+      <c r="B212" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C212" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D212" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>16</v>
-      </c>
-      <c r="C213" t="s">
-        <v>17</v>
-      </c>
-      <c r="D213" t="s">
-        <v>18</v>
-      </c>
+      <c r="A213" t="s">
+        <v>177</v>
+      </c>
+      <c r="B213" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="C213" s="6"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="B214" s="6">
-        <v>19.899999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="C214" s="6"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>154</v>
-      </c>
-      <c r="B215" s="6"/>
+        <v>179</v>
+      </c>
+      <c r="B215" s="6">
+        <v>86400</v>
+      </c>
       <c r="C215" s="6"/>
-      <c r="E215" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="B216" s="6">
-        <v>0.03</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C216" s="6"/>
-      <c r="E216" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="B217" s="6">
-        <v>3</v>
+        <v>0.24</v>
       </c>
       <c r="C217" s="6"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>158</v>
+        <v>2</v>
       </c>
       <c r="B218" s="6">
-        <v>1</v>
-      </c>
-      <c r="C218" s="6"/>
+        <v>0.99</v>
+      </c>
+      <c r="C218" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="D218" t="s">
+        <v>5</v>
+      </c>
+      <c r="E218" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
+        <v>3</v>
+      </c>
+      <c r="B219" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="C219" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D219" t="s">
+        <v>6</v>
+      </c>
+      <c r="E219" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>182</v>
+      </c>
+      <c r="B220" s="6">
+        <v>300</v>
+      </c>
+      <c r="C220" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E220" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>47</v>
+      </c>
+      <c r="B221" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C221" s="6"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>91</v>
+      </c>
+      <c r="B222" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>95</v>
+      </c>
+      <c r="B223" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="C223" s="6"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>63</v>
+      </c>
+      <c r="B224" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C224" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D224" t="s">
+        <v>7</v>
+      </c>
+      <c r="E224" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>64</v>
+      </c>
+      <c r="B225" s="6">
+        <v>50000</v>
+      </c>
+      <c r="C225" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D225" t="s">
+        <v>8</v>
+      </c>
+      <c r="E225" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>42</v>
       </c>
-      <c r="B219" s="6"/>
-      <c r="C219" s="6"/>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B220" s="6"/>
-      <c r="C220" s="6"/>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B227" s="6"/>
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B228" s="6"/>
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B223" t="s">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B230" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C223" s="6"/>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B224" s="6">
-        <v>1</v>
-      </c>
-      <c r="C224" s="6"/>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="6"/>
-      <c r="C225" s="6"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>16</v>
-      </c>
-      <c r="C226" t="s">
-        <v>17</v>
-      </c>
-      <c r="D226" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>166</v>
-      </c>
-      <c r="B227" s="6">
-        <v>100000</v>
-      </c>
-      <c r="C227" s="6"/>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>167</v>
-      </c>
-      <c r="B228" s="6">
-        <v>15</v>
-      </c>
-      <c r="C228" s="6"/>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>155</v>
-      </c>
-      <c r="B229" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="C229" s="6"/>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>168</v>
-      </c>
-      <c r="B230" s="6">
-        <v>3</v>
-      </c>
       <c r="C230" s="6"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>169</v>
-      </c>
-      <c r="B231" s="6">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B231" s="7">
         <v>1</v>
       </c>
       <c r="C231" s="6"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>42</v>
-      </c>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B233" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C233" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D233" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>1</v>
+      </c>
+      <c r="B234" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C234" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D234" t="s">
+        <v>5</v>
+      </c>
+      <c r="E234" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>111</v>
+      </c>
+      <c r="B235" s="6">
+        <v>2</v>
+      </c>
+      <c r="C235" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D235" t="s">
+        <v>113</v>
+      </c>
+      <c r="E235" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>2</v>
+      </c>
+      <c r="B236" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="C236" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="D236" t="s">
+        <v>5</v>
+      </c>
+      <c r="E236" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>3</v>
+      </c>
+      <c r="B237" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="C237" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D237" t="s">
+        <v>6</v>
+      </c>
+      <c r="E237" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>84</v>
+      </c>
+      <c r="B238" s="6">
+        <v>1</v>
+      </c>
+      <c r="C238" s="6">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
+        <v>85</v>
+      </c>
+      <c r="E238" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>182</v>
+      </c>
+      <c r="B239" s="6">
+        <v>300</v>
+      </c>
+      <c r="C239" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E239" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B240" s="6"/>
+      <c r="C240" s="6"/>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>95</v>
+      </c>
+      <c r="B241" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="C241" s="6"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>63</v>
+      </c>
+      <c r="B242" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C242" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D242" t="s">
+        <v>7</v>
+      </c>
+      <c r="E242" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>64</v>
+      </c>
+      <c r="B243" s="6">
+        <v>50000</v>
+      </c>
+      <c r="C243" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D243" t="s">
+        <v>8</v>
+      </c>
+      <c r="E243" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>42</v>
+      </c>
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B247" s="6"/>
+      <c r="C247" s="6"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B249" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B236">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B238" t="s">
+      <c r="C249" s="6"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B250" s="6">
+        <v>1</v>
+      </c>
+      <c r="C250" s="6"/>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B251" s="6"/>
+      <c r="C251" s="6"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
         <v>16</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C252" t="s">
         <v>17</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D252" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="9"/>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C244" s="6"/>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B245" s="6">
-        <v>1</v>
-      </c>
-      <c r="C245" s="6"/>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B246" s="6"/>
-      <c r="C246" s="6"/>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B247" t="s">
-        <v>16</v>
-      </c>
-      <c r="C247" t="s">
-        <v>17</v>
-      </c>
-      <c r="D247" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B248">
-        <v>0.25</v>
-      </c>
-      <c r="C248" s="6"/>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>42</v>
-      </c>
-      <c r="B249" s="6"/>
-      <c r="C249" s="6"/>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="1"/>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="2"/>
-      <c r="B251" s="7"/>
-      <c r="C251" s="6"/>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>15</v>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>153</v>
+      </c>
+      <c r="B253" s="6">
+        <v>19.899999999999999</v>
       </c>
       <c r="C253" s="6"/>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B254" s="6">
-        <v>1</v>
-      </c>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>154</v>
+      </c>
+      <c r="B254" s="6"/>
       <c r="C254" s="6"/>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="6"/>
+      <c r="E254" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>155</v>
+      </c>
+      <c r="B255" s="6">
+        <v>0.03</v>
+      </c>
       <c r="C255" s="6"/>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
-        <v>16</v>
-      </c>
-      <c r="C256" t="s">
-        <v>17</v>
-      </c>
-      <c r="D256" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B257">
-        <v>0.05</v>
+      <c r="E255" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>157</v>
+      </c>
+      <c r="B256" s="6">
+        <v>3</v>
+      </c>
+      <c r="C256" s="6"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>158</v>
+      </c>
+      <c r="B257" s="6">
+        <v>1</v>
       </c>
       <c r="C257" s="6"/>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>42</v>
       </c>
       <c r="B258" s="6"/>
       <c r="C258" s="6"/>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="4"/>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B259" s="6"/>
+      <c r="C259" s="6"/>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B262" t="s">
+        <v>15</v>
+      </c>
+      <c r="C262" s="6"/>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B263" s="6">
+        <v>1</v>
+      </c>
+      <c r="C263" s="6"/>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B264" s="6"/>
+      <c r="C264" s="6"/>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>16</v>
+      </c>
+      <c r="C265" t="s">
+        <v>17</v>
+      </c>
+      <c r="D265" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>166</v>
+      </c>
+      <c r="B266" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C266" s="6"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>167</v>
+      </c>
+      <c r="B267" s="6">
+        <v>15</v>
+      </c>
+      <c r="C267" s="6"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>155</v>
+      </c>
+      <c r="B268" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C268" s="6"/>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>168</v>
+      </c>
+      <c r="B269" s="6">
+        <v>1</v>
+      </c>
+      <c r="C269" s="6"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>169</v>
+      </c>
+      <c r="B270" s="6">
+        <v>10</v>
+      </c>
       <c r="C270" s="6"/>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="1"/>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="2"/>
-      <c r="B272" s="7"/>
-      <c r="C272" s="6"/>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="2"/>
-      <c r="B273" s="7"/>
-      <c r="C273" s="6"/>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B274" s="6"/>
-      <c r="C274" s="6"/>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B275" s="6"/>
-      <c r="C275" s="6"/>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B276" s="6"/>
-      <c r="C276" s="6"/>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B277" s="6"/>
-      <c r="C277" s="6"/>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B278" s="6"/>
-      <c r="C278" s="6"/>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B279" s="6"/>
-      <c r="C279" s="6"/>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B280" s="6"/>
-      <c r="C280" s="6"/>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B281" s="6"/>
-      <c r="C281" s="6"/>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B282" s="6"/>
-      <c r="C282" s="6"/>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B283" s="6"/>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>42</v>
+      </c>
+      <c r="B271" s="6"/>
+      <c r="C271" s="6"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>16</v>
+      </c>
+      <c r="C277" t="s">
+        <v>17</v>
+      </c>
+      <c r="D277" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B281" s="9"/>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C283" s="6"/>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B284" s="6"/>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B284" s="6">
+        <v>1</v>
+      </c>
       <c r="C284" s="6"/>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B285" s="6"/>
       <c r="C285" s="6"/>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B286" s="6"/>
-      <c r="C286" s="6"/>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B287" s="6"/>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>16</v>
+      </c>
+      <c r="C286" t="s">
+        <v>17</v>
+      </c>
+      <c r="D286" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B287">
+        <v>0.25</v>
+      </c>
       <c r="C287" s="6"/>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>42</v>
+      </c>
       <c r="B288" s="6"/>
       <c r="C288" s="6"/>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B289" s="6"/>
-      <c r="C289" s="6"/>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B290" s="6"/>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="1"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="2"/>
+      <c r="B290" s="7"/>
       <c r="C290" s="6"/>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B291" s="6"/>
-      <c r="C291" s="6"/>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B292" s="6"/>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C292" s="6"/>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B293" s="6"/>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B293" s="6">
+        <v>1</v>
+      </c>
       <c r="C293" s="6"/>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B296" s="6"/>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B295" t="s">
+        <v>16</v>
+      </c>
+      <c r="C295" t="s">
+        <v>17</v>
+      </c>
+      <c r="D295" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B296">
+        <v>0.05</v>
+      </c>
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>42</v>
+      </c>
       <c r="B297" s="6"/>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" s="1"/>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299" s="2"/>
-      <c r="B299" s="7"/>
-      <c r="C299" s="6"/>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" s="2"/>
-      <c r="B300" s="7"/>
-      <c r="C300" s="6"/>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B301" s="6"/>
-      <c r="C301" s="6"/>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B302" s="6"/>
-      <c r="C302" s="6"/>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B303" s="6"/>
-      <c r="C303" s="6"/>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B304" s="6"/>
-      <c r="C304" s="6"/>
-    </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B305" s="6"/>
-      <c r="C305" s="6"/>
-    </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B306" s="6"/>
-      <c r="C306" s="6"/>
-    </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B307" s="6"/>
-      <c r="C307" s="6"/>
-    </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B308" s="6"/>
-      <c r="C308" s="6"/>
-    </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B309" s="6"/>
+      <c r="C297" s="6"/>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" s="4"/>
       <c r="C309" s="6"/>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B310" s="6"/>
-      <c r="C310" s="6"/>
-    </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B311" s="6"/>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" s="2"/>
+      <c r="B311" s="7"/>
       <c r="C311" s="6"/>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B312" s="6"/>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="2"/>
+      <c r="B312" s="7"/>
       <c r="C312" s="6"/>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B313" s="6"/>
       <c r="C313" s="6"/>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B314" s="6"/>
       <c r="C314" s="6"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B315" s="6"/>
+      <c r="C315" s="6"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B316" s="6"/>
+      <c r="C316" s="6"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B317" s="6"/>
+      <c r="C317" s="6"/>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B318" s="6"/>
+      <c r="C318" s="6"/>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B319" s="6"/>
+      <c r="C319" s="6"/>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B320" s="6"/>
+      <c r="C320" s="6"/>
+    </row>
+    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B321" s="6"/>
+      <c r="C321" s="6"/>
+    </row>
+    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B322" s="6"/>
+      <c r="C322" s="6"/>
+    </row>
+    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B323" s="6"/>
+      <c r="C323" s="6"/>
+    </row>
+    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B324" s="6"/>
+      <c r="C324" s="6"/>
+    </row>
+    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B325" s="6"/>
+      <c r="C325" s="6"/>
+    </row>
+    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B326" s="6"/>
+      <c r="C326" s="6"/>
+    </row>
+    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B327" s="6"/>
+      <c r="C327" s="6"/>
+    </row>
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B328" s="6"/>
+      <c r="C328" s="6"/>
+    </row>
+    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B329" s="6"/>
+      <c r="C329" s="6"/>
+    </row>
+    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B330" s="6"/>
+      <c r="C330" s="6"/>
+    </row>
+    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B331" s="6"/>
+      <c r="C331" s="6"/>
+    </row>
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B332" s="6"/>
+      <c r="C332" s="6"/>
+    </row>
+    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B335" s="6"/>
+    </row>
+    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B336" s="6"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" s="1"/>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" s="2"/>
+      <c r="B338" s="7"/>
+      <c r="C338" s="6"/>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" s="2"/>
+      <c r="B339" s="7"/>
+      <c r="C339" s="6"/>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B340" s="6"/>
+      <c r="C340" s="6"/>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B341" s="6"/>
+      <c r="C341" s="6"/>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B342" s="6"/>
+      <c r="C342" s="6"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B343" s="6"/>
+      <c r="C343" s="6"/>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B344" s="6"/>
+      <c r="C344" s="6"/>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B345" s="6"/>
+      <c r="C345" s="6"/>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B346" s="6"/>
+      <c r="C346" s="6"/>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B347" s="6"/>
+      <c r="C347" s="6"/>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B348" s="6"/>
+      <c r="C348" s="6"/>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B349" s="6"/>
+      <c r="C349" s="6"/>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B350" s="6"/>
+      <c r="C350" s="6"/>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B351" s="6"/>
+      <c r="C351" s="6"/>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B352" s="6"/>
+      <c r="C352" s="6"/>
+    </row>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C353" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update hydraulic conductivity and LAT_WATER_RESERVOIR for SNOW
</commit_message>
<xml_diff>
--- a/results/example1/example1.xlsx
+++ b/results/example1/example1.xlsx
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
         <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
         <v>149</v>
@@ -1699,7 +1699,7 @@
         <v>107</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="C84" s="8"/>
     </row>
@@ -3217,7 +3217,7 @@
         <v>153</v>
       </c>
       <c r="B253" s="6">
-        <v>19.899999999999999</v>
+        <v>18</v>
       </c>
       <c r="C253" s="6"/>
     </row>
@@ -3248,7 +3248,7 @@
         <v>157</v>
       </c>
       <c r="B256" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C256" s="6"/>
     </row>
@@ -3257,7 +3257,7 @@
         <v>158</v>
       </c>
       <c r="B257" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C257" s="6"/>
     </row>

</xml_diff>

<commit_message>
error in LAT_SEEPAGE_FACE corrected + documentation uploaded
</commit_message>
<xml_diff>
--- a/results/example1/example1.xlsx
+++ b/results/example1/example1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="169">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -59,9 +59,6 @@
     <t>surface emissivity</t>
   </si>
   <si>
-    <t>height of air temperature</t>
-  </si>
-  <si>
     <t>roughness length</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>lower</t>
   </si>
   <si>
-    <t>geothermal heat flux</t>
-  </si>
-  <si>
     <t>TOP</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>geographical coordinates</t>
   </si>
   <si>
-    <t>a.s.l.</t>
-  </si>
-  <si>
     <t>domain_depth</t>
   </si>
   <si>
@@ -203,9 +194,6 @@
     <t>STRAT_linear</t>
   </si>
   <si>
-    <t>should match a GRID point, model domain extends to this depth</t>
-  </si>
-  <si>
     <t>dt_max</t>
   </si>
   <si>
@@ -245,9 +233,6 @@
     <t>[y]</t>
   </si>
   <si>
-    <t>if left empty, the entire output will be written out at the end</t>
-  </si>
-  <si>
     <t>provide in format dd.mm.yyyy; if left empty, the last timestamp of the forcing data set will be used</t>
   </si>
   <si>
@@ -404,12 +389,6 @@
     <t>CG_Beaufort_81_880_short.mat</t>
   </si>
   <si>
-    <t xml:space="preserve">area of the </t>
-  </si>
-  <si>
-    <t>OUT_all</t>
-  </si>
-  <si>
     <t>LATERAL_CLASS</t>
   </si>
   <si>
@@ -429,6 +408,129 @@
   </si>
   <si>
     <t>SUBSURFACE_CLASS</t>
+  </si>
+  <si>
+    <t>LATERAL_IA_CLASS</t>
+  </si>
+  <si>
+    <t>LAT_SEEPAGE_FACE_WATER</t>
+  </si>
+  <si>
+    <t>upperElevation</t>
+  </si>
+  <si>
+    <t>[m] a.s.l.</t>
+  </si>
+  <si>
+    <t>upper elevation of seepage face, set very high value instead of infinity</t>
+  </si>
+  <si>
+    <t>lowerElevation</t>
+  </si>
+  <si>
+    <t>lower elevation  of seepage face, set very low value instead of minus infinity</t>
+  </si>
+  <si>
+    <t>hardBottom_cutoff</t>
+  </si>
+  <si>
+    <t>threshold volumetric water content below which a grid cell is considered "hard", i.e. impermeable to water</t>
+  </si>
+  <si>
+    <t>distance_seepageFace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance to seepage face, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>seepage_contact_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lateral contact length of seepage face, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>LAT_WATER_RESERVOIR</t>
+  </si>
+  <si>
+    <t>reservoir_elevation</t>
+  </si>
+  <si>
+    <t>reservoir_temperature</t>
+  </si>
+  <si>
+    <t>water reservoir temperature  - if empty, water added at the temperature of the respective grid cell - only active for Xice classes</t>
+  </si>
+  <si>
+    <t>distance_reservoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance to water reservoir, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>reservoir_contact_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lateral contact length of water reservoir, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>LAT_REMOVE_SURFACE_WATER</t>
+  </si>
+  <si>
+    <t>NO_PARAMERTERS_REQUIRED</t>
+  </si>
+  <si>
+    <t>LAT_REMOVE_SUBSURFACE_WATER</t>
+  </si>
+  <si>
+    <t>list of LATERAL INTERACTION classes to be used for the run, must be initialized below</t>
+  </si>
+  <si>
+    <t>surface elevation a.s.l.</t>
+  </si>
+  <si>
+    <t>interval after which output file is written - if left empty, the entire output will be written out at the end</t>
+  </si>
+  <si>
+    <t>timestep of output</t>
+  </si>
+  <si>
+    <t>date of the year at which the output is written to an output file</t>
+  </si>
+  <si>
+    <t>name of the file with forcing data</t>
+  </si>
+  <si>
+    <t>vertical extent of the model domain - should match a GRID point</t>
+  </si>
+  <si>
+    <t>area of the model realization</t>
+  </si>
+  <si>
+    <t>geothermal heat flux at lower boundary</t>
+  </si>
+  <si>
+    <t>height at which air temperature is provided</t>
+  </si>
+  <si>
+    <t>OUT_all_lateral</t>
+  </si>
+  <si>
+    <t>[s/m]</t>
+  </si>
+  <si>
+    <t>surface restsinace against evapotranspiration</t>
+  </si>
+  <si>
+    <t>[degreee]</t>
+  </si>
+  <si>
+    <t>target SWE per grid cell</t>
+  </si>
+  <si>
+    <t>[day]</t>
+  </si>
+  <si>
+    <t>elevation of water reservoir</t>
   </si>
 </sst>
 </file>
@@ -771,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E188"/>
+  <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,179 +889,184 @@
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B5" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="D5" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
         <v>99</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="D7" t="s">
         <v>102</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>108</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>110</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>112</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>114</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" t="s">
         <v>118</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E14" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="B15">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,23 +1077,23 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -994,64 +1101,70 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B22">
         <v>0.25</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
         <v>67</v>
       </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
-        <v>71</v>
+      <c r="D23" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -1059,32 +1172,35 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="D32" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B33" s="5"/>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1093,12 +1209,12 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1107,37 +1223,37 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B39">
         <v>20</v>
@@ -1146,12 +1262,12 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>100</v>
@@ -1160,26 +1276,26 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B41">
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <v>0.05</v>
@@ -1188,12 +1304,12 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1202,30 +1318,30 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
@@ -1233,13 +1349,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,7 +1371,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1315,30 +1431,30 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" s="2">
         <v>1</v>
@@ -1346,246 +1462,246 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
-      <c r="B68">
-        <v>0.3</v>
+      <c r="B68" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="C68">
-        <v>0.5</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>0.5</v>
-      </c>
-      <c r="B69">
-        <v>0.5</v>
+        <v>10</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C69">
-        <v>0.5</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>10</v>
-      </c>
-      <c r="B70">
-        <v>0.97</v>
-      </c>
-      <c r="C70">
-        <v>0.03</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0.03</v>
-      </c>
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>32</v>
-      </c>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="4">
+        <v>1</v>
+      </c>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>0.3</v>
+      </c>
+      <c r="C83">
+        <v>0.5</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.5</v>
+      </c>
+      <c r="B84">
+        <v>0.5</v>
+      </c>
+      <c r="C84">
+        <v>0.5</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>0.03</v>
+      </c>
+      <c r="C85">
+        <v>0.97</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>0</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>10</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" s="4"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>91</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C85" s="8"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86" s="4">
-        <v>1</v>
-      </c>
-      <c r="C86" s="8"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B91" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="B93" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -1606,7 +1722,7 @@
         <v>2</v>
       </c>
       <c r="B98">
-        <v>-1</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,7 +1730,7 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -1627,30 +1743,30 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -1658,13 +1774,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" t="s">
         <v>16</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>17</v>
-      </c>
-      <c r="D109" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="B112">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C112">
         <v>1E-3</v>
@@ -1715,12 +1831,12 @@
         <v>6</v>
       </c>
       <c r="E112" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B113">
         <v>3600</v>
@@ -1732,12 +1848,12 @@
         <v>7</v>
       </c>
       <c r="E113" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B114">
         <v>50000</v>
@@ -1749,12 +1865,12 @@
         <v>8</v>
       </c>
       <c r="E114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B115" s="9">
         <v>1.0000000000000001E-5</v>
@@ -1762,7 +1878,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B116">
         <v>0.1</v>
@@ -1770,7 +1886,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B117">
         <v>0.1</v>
@@ -1778,7 +1894,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B118">
         <v>0.5</v>
@@ -1786,7 +1902,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -1794,20 +1910,20 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B124" s="7">
         <v>1</v>
@@ -1818,13 +1934,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B126" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="D126" t="s">
         <v>17</v>
-      </c>
-      <c r="D126" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,17 +1991,23 @@
         <v>6</v>
       </c>
       <c r="E129" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B130" s="6">
         <v>100</v>
       </c>
       <c r="C130" s="6"/>
+      <c r="D130" t="s">
+        <v>163</v>
+      </c>
+      <c r="E130" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -1903,7 +2025,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B132" s="6">
         <v>3600</v>
@@ -1915,12 +2037,12 @@
         <v>7</v>
       </c>
       <c r="E132" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B133" s="6">
         <v>50000</v>
@@ -1932,12 +2054,12 @@
         <v>8</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
@@ -1947,27 +2069,27 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C137" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137" t="s">
         <v>17</v>
-      </c>
-      <c r="D137" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B139" s="7">
         <v>1</v>
@@ -1980,31 +2102,40 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B141" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B142" s="6">
         <v>0</v>
       </c>
+      <c r="D142" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B143" s="6">
         <v>0.71</v>
       </c>
+      <c r="D143" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B144" s="6">
         <v>0.21</v>
+      </c>
+      <c r="D144" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,42 +2169,40 @@
         <v>6</v>
       </c>
       <c r="E146" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>80</v>
-      </c>
-      <c r="B147" s="6">
-        <v>0</v>
-      </c>
+      <c r="B147" s="6"/>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B148" s="6">
         <v>48</v>
       </c>
       <c r="C148" s="6"/>
       <c r="D148" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B149" s="6">
         <v>0.05</v>
       </c>
       <c r="C149" s="6"/>
+      <c r="D149" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B150" s="9">
         <v>1E-4</v>
@@ -2082,16 +2211,22 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B151" s="6">
         <v>0.02</v>
       </c>
       <c r="C151" s="6"/>
+      <c r="D151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E151" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B152" s="6">
         <v>3600</v>
@@ -2103,12 +2238,12 @@
         <v>7</v>
       </c>
       <c r="E152" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B153" s="6">
         <v>50000</v>
@@ -2120,7 +2255,7 @@
         <v>8</v>
       </c>
       <c r="E153" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -2129,7 +2264,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
@@ -2144,145 +2279,404 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C159" s="6"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B160" s="7">
         <v>1</v>
       </c>
       <c r="C160" s="6"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B162" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C162" s="6" t="s">
+      <c r="D162" t="s">
         <v>17</v>
       </c>
-      <c r="D162" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B163" s="6">
         <v>0.25</v>
       </c>
       <c r="C163" s="6"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="6"/>
-      <c r="C167" s="6"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B169" s="6">
+        <v>1</v>
+      </c>
+      <c r="C169" s="6"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="6"/>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="2"/>
-      <c r="B173" s="7"/>
+      <c r="C170" s="6"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>15</v>
+      </c>
+      <c r="C171" t="s">
+        <v>16</v>
+      </c>
+      <c r="D171" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>130</v>
+      </c>
+      <c r="B172" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C172" s="6"/>
+      <c r="D172" t="s">
+        <v>131</v>
+      </c>
+      <c r="E172" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>133</v>
+      </c>
+      <c r="B173" s="6">
+        <v>15</v>
+      </c>
       <c r="C173" s="6"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="2"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="6"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="6"/>
+      <c r="D173" t="s">
+        <v>131</v>
+      </c>
+      <c r="E173" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>135</v>
+      </c>
+      <c r="B174" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C174" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D174" t="s">
+        <v>5</v>
+      </c>
+      <c r="E174" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>137</v>
+      </c>
+      <c r="B175" s="6">
+        <v>10</v>
+      </c>
       <c r="C175" s="6"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="6"/>
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>139</v>
+      </c>
+      <c r="B176" s="6">
+        <v>10</v>
+      </c>
       <c r="C176" s="6"/>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>6</v>
+      </c>
+      <c r="E176" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>37</v>
+      </c>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B180" s="6"/>
-      <c r="C180" s="6"/>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" s="6"/>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B181" t="s">
+        <v>14</v>
+      </c>
       <c r="C181" s="6"/>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B182" s="6"/>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B182" s="6">
+        <v>1</v>
+      </c>
       <c r="C182" s="6"/>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B184" s="6"/>
-      <c r="C184" s="6"/>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B185" s="6"/>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" t="s">
+        <v>16</v>
+      </c>
+      <c r="D184" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>142</v>
+      </c>
+      <c r="B185" s="6">
+        <v>18</v>
+      </c>
       <c r="C185" s="6"/>
-    </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>131</v>
+      </c>
+      <c r="E185" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>143</v>
+      </c>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
-    </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B187" s="6"/>
-      <c r="C187" s="6"/>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D186" t="s">
+        <v>24</v>
+      </c>
+      <c r="E186" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>135</v>
+      </c>
+      <c r="B187" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C187" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D187" t="s">
+        <v>5</v>
+      </c>
+      <c r="E187" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>145</v>
+      </c>
+      <c r="B188" s="6">
+        <v>10</v>
+      </c>
       <c r="C188" s="6"/>
+      <c r="D188" t="s">
+        <v>6</v>
+      </c>
+      <c r="E188" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>147</v>
+      </c>
+      <c r="B189" s="6">
+        <v>10</v>
+      </c>
+      <c r="C189" s="6"/>
+      <c r="D189" t="s">
+        <v>6</v>
+      </c>
+      <c r="E189" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>37</v>
+      </c>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" t="s">
+        <v>16</v>
+      </c>
+      <c r="D197" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>15</v>
+      </c>
+      <c r="C206" t="s">
+        <v>16</v>
+      </c>
+      <c r="D206" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>